<commit_message>
incorporate linear scaling equation
</commit_message>
<xml_diff>
--- a/code/WLS_MQTT_toAdafruitIO_v6_STABLE/Pressure Sensor Calibration AIO Data/Pressure Sensor Calibration.xlsx
+++ b/code/WLS_MQTT_toAdafruitIO_v6_STABLE/Pressure Sensor Calibration AIO Data/Pressure Sensor Calibration.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frazerss\Documents\Arduino\Pressure Sensor Calibration AIO Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SmithCA\Documents\GitHub\DHEC-Stage-Sensor\code\WLS_MQTT_toAdafruitIO_v6_STABLE\Pressure Sensor Calibration AIO Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B31BCA76-3432-40A1-A5EA-F3C20C8A4D2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C70DA5-6E66-4CE9-95B3-619765AFC210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3105" windowWidth="21600" windowHeight="11385" xr2:uid="{E545EA9D-E698-426F-B9AF-EE7411AEA94E}"/>
+    <workbookView xWindow="-19320" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{E545EA9D-E698-426F-B9AF-EE7411AEA94E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Depth</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>depth-equivalent PSI</t>
+  </si>
+  <si>
+    <t>experimental voltage</t>
+  </si>
+  <si>
+    <t>experimental psi</t>
+  </si>
+  <si>
+    <t>experimental feet of water</t>
   </si>
 </sst>
 </file>
@@ -116,6 +126,3412 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="525203944"/>
+        <c:axId val="387465808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="525203944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="387465808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="387465808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525203944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>voltage to psi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1052101924759405"/>
+                  <c:y val="-3.3541119860017498E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>6.8528138528138527</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4935064935064934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0606060606060606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6277056277056277</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1948051948051948</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7619047619047619</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.329004329004329</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8961038961038961</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4632034632034632</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0303030303030303</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5974025974025974</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2186147186147185</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1645021645021645</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7316017316017316</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2987012987012987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.86580086580086579</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4329004329004329</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5875-40C8-8F36-96C57A8B75C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5875-40C8-8F36-96C57A8B75C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="758610896"/>
+        <c:axId val="763601096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="758610896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763601096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="763601096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>psi</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="758610896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>voltage to ft</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> water</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1052101924759405"/>
+                  <c:y val="-3.3541119860017498E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>15.822913048340547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.99328463203463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.993732323232322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.994180014430013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.994627705627705</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.995075396825396</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9955230880230879</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9959707792207784</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9964184704184698</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.9968661616161612</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.9973138528138525</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1227055826118315</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.9977615440115439</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.9982092352092349</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9986569264069263</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9991046176046174</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99955230880230872</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F3BD-448F-B05D-D8C5CB845726}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.089658333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F3BD-448F-B05D-D8C5CB845726}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="758610896"/>
+        <c:axId val="763601096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="758610896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763601096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="763601096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ft</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of water</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="758610896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114FEEB6-31DC-4113-94FB-E5C5E880810D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>909637</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B2CDF7-3053-4F23-9138-5B051A4DA23F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B36E275-3A54-432D-9420-F05EDD49DE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +3834,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,5 +4581,274 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9E5A91-021F-48F6-A3BE-3731BC6CA319}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.12</v>
+      </c>
+      <c r="B2">
+        <v>6.8528138528138527</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C18" si="0">B2*(27.70759/12)</f>
+        <v>15.822913048340547</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.98</v>
+      </c>
+      <c r="B3">
+        <v>6.4935064935064934</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>14.99328463203463</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.81</v>
+      </c>
+      <c r="B4">
+        <v>6.0606060606060606</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>13.993732323232322</v>
+      </c>
+      <c r="E4">
+        <f>E3*(27.70759/12)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>F3*(27.70759/12)</f>
+        <v>23.089658333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.64</v>
+      </c>
+      <c r="B5">
+        <v>5.6277056277056277</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>12.994180014430013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.48</v>
+      </c>
+      <c r="B6">
+        <v>5.1948051948051948</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>11.994627705627705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B7">
+        <v>4.7619047619047619</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>10.995075396825396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.13</v>
+      </c>
+      <c r="B8">
+        <v>4.329004329004329</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9.9955230880230879</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.96</v>
+      </c>
+      <c r="B9">
+        <v>3.8961038961038961</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8.9959707792207784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.79</v>
+      </c>
+      <c r="B10">
+        <v>3.4632034632034632</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7.9964184704184698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.61</v>
+      </c>
+      <c r="B11">
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>6.9968661616161612</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.44</v>
+      </c>
+      <c r="B12">
+        <v>2.5974025974025974</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5.9973138528138525</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="B13">
+        <v>2.2186147186147185</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5.1227055826118315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.27</v>
+      </c>
+      <c r="B14">
+        <v>2.1645021645021645</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>4.9977615440115439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="B15">
+        <v>1.7316017316017316</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.9982092352092349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.91</v>
+      </c>
+      <c r="B16">
+        <v>1.2987012987012987</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2.9986569264069263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.74</v>
+      </c>
+      <c r="B17">
+        <v>0.86580086580086579</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1.9991046176046174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B18">
+        <v>0.4329004329004329</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.99955230880230872</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.38</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>B19*(27.70759/12)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>